<commit_message>
rerun jhou to qc runway
</commit_message>
<xml_diff>
--- a/Bonnie's Codes/CREATE/runway_c01_16_mismatchfilenums.xlsx
+++ b/Bonnie's Codes/CREATE/runway_c01_16_mismatchfilenums.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t xml:space="preserve">cohort</t>
   </si>
@@ -35,12 +35,6 @@
     <t xml:space="preserve">C02</t>
   </si>
   <si>
-    <t xml:space="preserve">U25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U26</t>
-  </si>
-  <si>
     <t xml:space="preserve">U27</t>
   </si>
   <si>
@@ -69,6 +63,33 @@
   </si>
   <si>
     <t xml:space="preserve">C04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U99</t>
   </si>
   <si>
     <t xml:space="preserve">U110</t>
@@ -844,11 +865,9 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>7</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -861,38 +880,40 @@
         <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" t="n">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -906,7 +927,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -920,7 +941,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -934,324 +955,320 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" t="n">
         <v>7</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="n">
         <v>7</v>
       </c>
-      <c r="D12" t="n">
-        <v>6</v>
-      </c>
+      <c r="D12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" t="n">
         <v>7</v>
       </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
+      <c r="D17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" t="n">
-        <v>12</v>
-      </c>
-      <c r="D19" t="n">
-        <v>24</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
-        <v>12</v>
-      </c>
-      <c r="D20" t="n">
-        <v>24</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
       <c r="C21" t="n">
-        <v>7</v>
-      </c>
-      <c r="D21" t="n">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
-      </c>
-      <c r="D22" t="n">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" t="n">
-        <v>11</v>
-      </c>
-      <c r="D23" t="n">
-        <v>12</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D24" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
-      </c>
-      <c r="D25" t="n">
-        <v>10</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
       <c r="C26" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
       </c>
       <c r="C27" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D27" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="B28" t="s">
-        <v>38</v>
-      </c>
       <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28"/>
+        <v>7</v>
+      </c>
+      <c r="D28" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D29" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30"/>
+        <v>11</v>
+      </c>
+      <c r="D30" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31"/>
+        <v>12</v>
+      </c>
+      <c r="D31" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32"/>
+        <v>9</v>
+      </c>
+      <c r="D32" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33"/>
+        <v>11</v>
+      </c>
+      <c r="D33" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34"/>
+        <v>11</v>
+      </c>
+      <c r="D34" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1263,123 +1280,111 @@
         <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36"/>
+        <v>11</v>
+      </c>
+      <c r="D36" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
-      <c r="D37" t="n">
-        <v>5</v>
-      </c>
+      <c r="D37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C38" t="n">
-        <v>12</v>
-      </c>
-      <c r="D38" t="n">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" t="n">
-        <v>12</v>
-      </c>
-      <c r="D39" t="n">
-        <v>11</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" t="n">
-        <v>12</v>
-      </c>
-      <c r="D40" t="n">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" t="n">
-        <v>12</v>
-      </c>
-      <c r="D41" t="n">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" t="n">
-        <v>12</v>
-      </c>
-      <c r="D42" t="n">
-        <v>22</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
         <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" t="n">
-        <v>12</v>
-      </c>
-      <c r="D43" t="n">
-        <v>24</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
         <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1387,13 +1392,13 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" t="n">
         <v>12</v>
       </c>
       <c r="D45" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
@@ -1401,18 +1406,18 @@
         <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" t="n">
         <v>12</v>
       </c>
       <c r="D46" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>59</v>
@@ -1426,7 +1431,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
         <v>60</v>
@@ -1435,12 +1440,12 @@
         <v>12</v>
       </c>
       <c r="D48" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
         <v>61</v>
@@ -1449,12 +1454,12 @@
         <v>12</v>
       </c>
       <c r="D49" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
         <v>62</v>
@@ -1463,12 +1468,12 @@
         <v>12</v>
       </c>
       <c r="D50" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
         <v>63</v>
@@ -1482,7 +1487,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
         <v>64</v>
@@ -1491,12 +1496,12 @@
         <v>12</v>
       </c>
       <c r="D52" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
         <v>65</v>
@@ -1505,12 +1510,12 @@
         <v>12</v>
       </c>
       <c r="D53" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
         <v>66</v>
@@ -1519,12 +1524,12 @@
         <v>12</v>
       </c>
       <c r="D54" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
         <v>67</v>
@@ -1533,12 +1538,12 @@
         <v>12</v>
       </c>
       <c r="D55" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>68</v>
@@ -1547,57 +1552,57 @@
         <v>12</v>
       </c>
       <c r="D56" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
         <v>69</v>
       </c>
-      <c r="B57" t="s">
-        <v>70</v>
-      </c>
       <c r="C57" t="n">
         <v>12</v>
       </c>
       <c r="D57" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C58" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D58" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D59" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C60" t="n">
         <v>12</v>
@@ -1608,105 +1613,105 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C61" t="n">
         <v>12</v>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C62" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D62" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C63" t="n">
         <v>12</v>
       </c>
       <c r="D63" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
         <v>77</v>
       </c>
       <c r="C64" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D64" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
         <v>78</v>
       </c>
       <c r="C65" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D65" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
         <v>79</v>
       </c>
       <c r="C66" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B67" t="s">
         <v>80</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D67" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
         <v>81</v>
@@ -1720,367 +1725,367 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" t="s">
         <v>82</v>
       </c>
-      <c r="B69" t="s">
-        <v>83</v>
-      </c>
       <c r="C69" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D69" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C70" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D70" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C71" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D71" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" t="s">
         <v>85</v>
       </c>
-      <c r="B72" t="s">
-        <v>87</v>
-      </c>
       <c r="C72" t="n">
         <v>12</v>
       </c>
       <c r="D72" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C73" t="n">
         <v>12</v>
       </c>
       <c r="D73" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C74" t="n">
-        <v>12</v>
-      </c>
-      <c r="D74"/>
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C75" t="n">
         <v>12</v>
       </c>
       <c r="D75" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D76" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C77" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D77" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
         <v>93</v>
       </c>
       <c r="C78" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D78" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B79" t="s">
         <v>94</v>
       </c>
       <c r="C79" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D79" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B80" t="s">
         <v>95</v>
       </c>
       <c r="C80" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D80" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B81" t="s">
         <v>96</v>
       </c>
       <c r="C81" t="n">
-        <v>4</v>
-      </c>
-      <c r="D81" t="n">
-        <v>8</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
         <v>97</v>
       </c>
       <c r="C82" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D82" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>98</v>
       </c>
       <c r="C83" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D83" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B84" t="s">
         <v>99</v>
       </c>
       <c r="C84" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D84" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" t="s">
         <v>100</v>
       </c>
-      <c r="B85" t="s">
-        <v>101</v>
-      </c>
       <c r="C85" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D85" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C86" t="n">
         <v>11</v>
       </c>
       <c r="D86" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
-      </c>
-      <c r="D87"/>
+        <v>11</v>
+      </c>
+      <c r="D87" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C88" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D88" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C89" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D89" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C90" t="n">
         <v>7</v>
       </c>
       <c r="D90" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C91" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D91" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B92" t="s">
         <v>108</v>
       </c>
       <c r="C92" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D92" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B93" t="s">
         <v>109</v>
       </c>
       <c r="C93" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D93" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B94" t="s">
         <v>110</v>
       </c>
       <c r="C94" t="n">
-        <v>12</v>
-      </c>
-      <c r="D94" t="n">
-        <v>11</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D94"/>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s">
         <v>111</v>
@@ -2094,7 +2099,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B96" t="s">
         <v>112</v>
@@ -2108,13 +2113,13 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B97" t="s">
         <v>113</v>
       </c>
       <c r="C97" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D97" t="n">
         <v>9</v>
@@ -2122,271 +2127,275 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B98" t="s">
         <v>114</v>
       </c>
       <c r="C98" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D98" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B99" t="s">
         <v>115</v>
       </c>
       <c r="C99" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D99" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B100" t="s">
         <v>116</v>
       </c>
       <c r="C100" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D100" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B101" t="s">
         <v>117</v>
       </c>
       <c r="C101" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D101" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B102" t="s">
         <v>118</v>
       </c>
       <c r="C102" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D102" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B103" t="s">
         <v>119</v>
       </c>
       <c r="C103" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D103" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B104" t="s">
         <v>120</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D104" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B105" t="s">
         <v>121</v>
       </c>
       <c r="C105" t="n">
-        <v>9</v>
-      </c>
-      <c r="D105"/>
+        <v>6</v>
+      </c>
+      <c r="D105" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B106" t="s">
         <v>122</v>
       </c>
       <c r="C106" t="n">
+        <v>8</v>
+      </c>
+      <c r="D106" t="n">
         <v>9</v>
       </c>
-      <c r="D106"/>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B107" t="s">
         <v>123</v>
       </c>
       <c r="C107" t="n">
+        <v>5</v>
+      </c>
+      <c r="D107" t="n">
         <v>7</v>
       </c>
-      <c r="D107"/>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>124</v>
       </c>
       <c r="C108" t="n">
-        <v>8</v>
-      </c>
-      <c r="D108"/>
+        <v>11</v>
+      </c>
+      <c r="D108" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B109" t="s">
         <v>125</v>
       </c>
       <c r="C109" t="n">
-        <v>0</v>
-      </c>
-      <c r="D109"/>
+        <v>11</v>
+      </c>
+      <c r="D109" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B110" t="s">
         <v>126</v>
       </c>
       <c r="C110" t="n">
-        <v>7</v>
-      </c>
-      <c r="D110"/>
+        <v>10</v>
+      </c>
+      <c r="D110" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
+        <v>107</v>
+      </c>
+      <c r="B111" t="s">
         <v>127</v>
       </c>
-      <c r="B111" t="s">
-        <v>128</v>
-      </c>
       <c r="C111" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C112" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D112"/>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B113" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C113" t="n">
-        <v>10</v>
-      </c>
-      <c r="D113" t="n">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D113"/>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B114" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C114" t="n">
-        <v>12</v>
-      </c>
-      <c r="D114" t="n">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D114"/>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B115" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C115" t="n">
-        <v>12</v>
-      </c>
-      <c r="D115" t="n">
-        <v>13</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D115"/>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C116" t="n">
-        <v>12</v>
-      </c>
-      <c r="D116" t="n">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D116"/>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B117" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C117" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D117"/>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B118" t="s">
         <v>135</v>
@@ -2395,40 +2404,38 @@
         <v>12</v>
       </c>
       <c r="D118" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B119" t="s">
         <v>136</v>
       </c>
       <c r="C119" t="n">
-        <v>12</v>
-      </c>
-      <c r="D119" t="n">
-        <v>14</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D119"/>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B120" t="s">
         <v>137</v>
       </c>
       <c r="C120" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D120" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B121" t="s">
         <v>138</v>
@@ -2437,12 +2444,12 @@
         <v>12</v>
       </c>
       <c r="D121" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B122" t="s">
         <v>139</v>
@@ -2456,7 +2463,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B123" t="s">
         <v>140</v>
@@ -2465,26 +2472,24 @@
         <v>12</v>
       </c>
       <c r="D123" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B124" t="s">
         <v>141</v>
       </c>
       <c r="C124" t="n">
-        <v>12</v>
-      </c>
-      <c r="D124" t="n">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D124"/>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B125" t="s">
         <v>142</v>
@@ -2493,12 +2498,12 @@
         <v>12</v>
       </c>
       <c r="D125" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B126" t="s">
         <v>143</v>
@@ -2507,12 +2512,12 @@
         <v>12</v>
       </c>
       <c r="D126" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B127" t="s">
         <v>144</v>
@@ -2521,12 +2526,12 @@
         <v>12</v>
       </c>
       <c r="D127" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B128" t="s">
         <v>145</v>
@@ -2535,12 +2540,12 @@
         <v>12</v>
       </c>
       <c r="D128" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B129" t="s">
         <v>146</v>
@@ -2554,19 +2559,21 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B130" t="s">
         <v>147</v>
       </c>
       <c r="C130" t="n">
-        <v>1</v>
-      </c>
-      <c r="D130"/>
+        <v>12</v>
+      </c>
+      <c r="D130" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B131" t="s">
         <v>148</v>
@@ -2575,12 +2582,12 @@
         <v>12</v>
       </c>
       <c r="D131" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B132" t="s">
         <v>149</v>
@@ -2594,7 +2601,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B133" t="s">
         <v>150</v>
@@ -2603,6 +2610,102 @@
         <v>12</v>
       </c>
       <c r="D133" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C134" t="n">
+        <v>12</v>
+      </c>
+      <c r="D134" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>152</v>
+      </c>
+      <c r="C135" t="n">
+        <v>12</v>
+      </c>
+      <c r="D135" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>153</v>
+      </c>
+      <c r="C136" t="n">
+        <v>12</v>
+      </c>
+      <c r="D136" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>134</v>
+      </c>
+      <c r="B137" t="s">
+        <v>154</v>
+      </c>
+      <c r="C137" t="n">
+        <v>1</v>
+      </c>
+      <c r="D137"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>134</v>
+      </c>
+      <c r="B138" t="s">
+        <v>155</v>
+      </c>
+      <c r="C138" t="n">
+        <v>12</v>
+      </c>
+      <c r="D138" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>134</v>
+      </c>
+      <c r="B139" t="s">
+        <v>156</v>
+      </c>
+      <c r="C139" t="n">
+        <v>12</v>
+      </c>
+      <c r="D139" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>134</v>
+      </c>
+      <c r="B140" t="s">
+        <v>157</v>
+      </c>
+      <c r="C140" t="n">
+        <v>12</v>
+      </c>
+      <c r="D140" t="n">
         <v>11</v>
       </c>
     </row>

</xml_diff>